<commit_message>
Updated 24V load test data for Slot cards
</commit_message>
<xml_diff>
--- a/Test Data/Verify_24V_Load_On_Addition_Deletion_Of_Slot_Cards.xlsx
+++ b/Test Data/Verify_24V_Load_On_Addition_Deletion_Of_Slot_Cards.xlsx
@@ -600,7 +600,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,7 +765,7 @@
         <v>1.101</v>
       </c>
       <c r="O8" s="3">
-        <v>0.32900000000000001</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="P8" s="16" t="s">
         <v>44</v>

</xml_diff>